<commit_message>
srcl updated profile, Mymensingh PWD FS, AN Affairs BS
</commit_message>
<xml_diff>
--- a/Bill/Bill_Database.xlsx
+++ b/Bill/Bill_Database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SRCL\Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77C4DB33-F2F1-4711-BE18-DB593FD1B274}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{049170F9-3B31-4EDE-9DCC-C5FB528A67ED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="51">
   <si>
     <t>Date</t>
   </si>
@@ -145,6 +145,78 @@
   </si>
   <si>
     <t>Food</t>
+  </si>
+  <si>
+    <t>Jakir</t>
+  </si>
+  <si>
+    <t>Printing + Others</t>
+  </si>
+  <si>
+    <t>Printing + Banner</t>
+  </si>
+  <si>
+    <t>File Rack</t>
+  </si>
+  <si>
+    <t>Biscuit</t>
+  </si>
+  <si>
+    <t>Print</t>
+  </si>
+  <si>
+    <t>Print + Photocopy</t>
+  </si>
+  <si>
+    <t>File Purchase</t>
+  </si>
+  <si>
+    <t>Tea</t>
+  </si>
+  <si>
+    <t>Print +Banner + Uber</t>
+  </si>
+  <si>
+    <t>Tape</t>
+  </si>
+  <si>
+    <t>Print + Spiral</t>
+  </si>
+  <si>
+    <t>Photocopy + Spiral</t>
+  </si>
+  <si>
+    <t>Transport + Doi</t>
+  </si>
+  <si>
+    <t>Auto Seal</t>
+  </si>
+  <si>
+    <t>Courier + Recharge</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Tissue + Marker</t>
+  </si>
+  <si>
+    <t>File + Envelope</t>
+  </si>
+  <si>
+    <t>Van</t>
+  </si>
+  <si>
+    <t>A4 Paper</t>
+  </si>
+  <si>
+    <t>Sandal + Bin</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>Juthi Apa (L)</t>
   </si>
 </sst>
 </file>
@@ -215,7 +287,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -250,9 +322,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -702,7 +771,7 @@
   <dimension ref="A1:F50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7:H7"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -778,83 +847,181 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
+      <c r="A5" s="6">
+        <v>44140</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" s="2">
+        <v>605</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
+      <c r="A6" s="6">
+        <v>44145</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" s="2">
+        <v>500</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="A7" s="6">
+        <v>44154</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="A8" s="6">
+        <v>44156</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="2">
+        <v>1120</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="A9" s="6">
+        <v>44171</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
+      <c r="A10" s="6">
+        <v>44172</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2">
+        <v>500</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
+      <c r="A11" s="6">
+        <v>44173</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="B12" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="2">
+        <v>6250</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="6">
+        <v>44180</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
+      <c r="A14" s="6">
+        <v>44182</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2">
+        <v>1000</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1160,8 +1327,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05325F8F-BEEC-4CC8-B184-0C8693CC2175}">
   <dimension ref="A1:E50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1215,9 +1382,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8">
-        <v>44138</v>
-      </c>
+      <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1233,7 +1398,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="8">
-        <v>44138</v>
+        <v>44139</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -1249,9 +1414,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
-        <v>44139</v>
-      </c>
+      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1266,7 +1429,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13">
+      <c r="A7" s="8">
         <v>44140</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -1283,199 +1446,393 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="A8" s="8">
+        <v>44141</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="2">
+        <v>65</v>
+      </c>
+      <c r="D8" s="2">
+        <v>70</v>
+      </c>
       <c r="E8" s="2"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
+      <c r="A9" s="8">
+        <v>44143</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="2">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2">
+        <v>40</v>
+      </c>
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
+      <c r="A10" s="8">
+        <v>44144</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="2">
+        <v>100</v>
+      </c>
+      <c r="D10" s="2">
+        <v>440</v>
+      </c>
       <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
+      <c r="A11" s="8">
+        <v>44145</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="2">
+        <v>135</v>
+      </c>
+      <c r="D11" s="2">
+        <v>305</v>
+      </c>
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="8"/>
+      <c r="B12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="2">
+        <v>150</v>
+      </c>
+      <c r="D12" s="2">
+        <v>155</v>
+      </c>
       <c r="E12" s="2"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="A13" s="8"/>
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="2">
+        <v>30</v>
+      </c>
+      <c r="D13" s="2">
+        <v>125</v>
+      </c>
       <c r="E13" s="2"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="A14" s="8">
+        <v>44147</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C14" s="2">
+        <v>50</v>
+      </c>
+      <c r="D14" s="2">
+        <v>75</v>
+      </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
+      <c r="A15" s="8">
+        <v>44156</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C15" s="2">
+        <v>660</v>
+      </c>
+      <c r="D15" s="2">
+        <v>415</v>
+      </c>
       <c r="E15" s="2"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1120</v>
+      </c>
+      <c r="D16" s="2">
+        <v>415</v>
+      </c>
       <c r="E16" s="2"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
+      <c r="A17" s="8">
+        <v>44158</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" s="2">
+        <v>275</v>
+      </c>
+      <c r="D17" s="2">
+        <v>140</v>
+      </c>
       <c r="E17" s="2"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="2">
+        <v>80</v>
+      </c>
+      <c r="D18" s="2">
+        <v>60</v>
+      </c>
       <c r="E18" s="2"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
+      <c r="A19" s="8">
+        <v>44171</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19" s="2">
+        <v>790</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1270</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="2">
+        <v>680</v>
+      </c>
+      <c r="D20" s="2">
+        <v>590</v>
+      </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
+      <c r="A21" s="8"/>
+      <c r="B21" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="2">
+        <v>205</v>
+      </c>
+      <c r="D21" s="2">
+        <v>385</v>
+      </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="2"/>
-      <c r="D22" s="2"/>
+      <c r="A22" s="8">
+        <v>44172</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C22" s="2">
+        <v>220</v>
+      </c>
+      <c r="D22" s="2">
+        <v>665</v>
+      </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
+      <c r="A23" s="8"/>
+      <c r="B23" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C23" s="2">
+        <v>330</v>
+      </c>
+      <c r="D23" s="2">
+        <v>335</v>
+      </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
+      <c r="A24" s="8"/>
+      <c r="B24" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C24" s="2">
+        <v>230</v>
+      </c>
+      <c r="D24" s="2">
+        <v>105</v>
+      </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="2"/>
-      <c r="D25" s="2"/>
+      <c r="A25" s="8">
+        <v>44174</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="2">
+        <v>850</v>
+      </c>
+      <c r="D25" s="2">
+        <v>255</v>
+      </c>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C26" s="2">
+        <v>130</v>
+      </c>
+      <c r="D26" s="2">
+        <v>125</v>
+      </c>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C27" s="2">
+        <v>120</v>
+      </c>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
       <c r="E27" s="2"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2"/>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C28" s="2">
+        <v>310</v>
+      </c>
+      <c r="D28" s="2">
+        <v>-305</v>
+      </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
+      <c r="A29" s="8">
+        <v>44177</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="2">
+        <v>6000</v>
+      </c>
+      <c r="D29" s="2">
+        <v>-55</v>
+      </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C30" s="2">
+        <v>700</v>
+      </c>
+      <c r="D30" s="2">
+        <v>-755</v>
+      </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C31" s="2">
+        <v>80</v>
+      </c>
+      <c r="D31" s="2">
+        <v>-835</v>
+      </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
+      <c r="A32" s="8">
+        <v>44180</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="2">
+        <v>150</v>
+      </c>
+      <c r="D32" s="2">
+        <v>-315</v>
+      </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2"/>
-      <c r="C33" s="2"/>
-      <c r="D33" s="2"/>
+      <c r="A33" s="8">
+        <v>44182</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C33" s="2">
+        <v>225</v>
+      </c>
+      <c r="D33" s="2">
+        <v>-540</v>
+      </c>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="2"/>
-      <c r="D34" s="2"/>
+      <c r="A34" s="8"/>
+      <c r="B34" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C34" s="2">
+        <v>390</v>
+      </c>
+      <c r="D34" s="2">
+        <v>-930</v>
+      </c>
       <c r="E34" s="2"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
-      <c r="C35" s="2"/>
-      <c r="D35" s="2"/>
+      <c r="A35" s="8"/>
+      <c r="B35" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="2">
+        <v>200</v>
+      </c>
+      <c r="D35" s="2">
+        <v>-130</v>
+      </c>
       <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,7 +1954,7 @@
   <dimension ref="A1:E50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,9 +2008,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="9">
-        <v>44077</v>
-      </c>
+      <c r="A4" s="9"/>
       <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
@@ -1668,9 +2023,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="9">
-        <v>44077</v>
-      </c>
+      <c r="A5" s="9"/>
       <c r="B5" s="3" t="s">
         <v>19</v>
       </c>
@@ -1685,9 +2038,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="9">
-        <v>44077</v>
-      </c>
+      <c r="A6" s="9"/>
       <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
@@ -1719,9 +2070,7 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9">
-        <v>44107</v>
-      </c>
+      <c r="A8" s="9"/>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
@@ -1736,9 +2085,7 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="9">
-        <v>44107</v>
-      </c>
+      <c r="A9" s="9"/>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
@@ -1753,9 +2100,7 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9">
-        <v>44107</v>
-      </c>
+      <c r="A10" s="9"/>
       <c r="B10" s="3" t="s">
         <v>23</v>
       </c>
@@ -1787,9 +2132,7 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9">
-        <v>44138</v>
-      </c>
+      <c r="A12" s="9"/>
       <c r="B12" s="3" t="s">
         <v>24</v>
       </c>
@@ -1804,9 +2147,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="9">
-        <v>44138</v>
-      </c>
+      <c r="A13" s="9"/>
       <c r="B13" s="3" t="s">
         <v>24</v>
       </c>
@@ -1821,9 +2162,7 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="9">
-        <v>44138</v>
-      </c>
+      <c r="A14" s="9"/>
       <c r="B14" s="3" t="s">
         <v>24</v>
       </c>
@@ -1838,9 +2177,7 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="9">
-        <v>44138</v>
-      </c>
+      <c r="A15" s="9"/>
       <c r="B15" s="3" t="s">
         <v>24</v>
       </c>
@@ -1855,39 +2192,83 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="A16" s="9">
+        <v>44141</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
-      <c r="B17" s="3"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
+      <c r="A17" s="9">
+        <v>44172</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C17" s="3">
+        <v>50000</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="3">
+        <v>35000</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="9"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C19" s="3">
+        <v>12000</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="9"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C20" s="3">
+        <v>3000</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="9"/>

</xml_diff>

<commit_message>
Bill database, Jail proposal updated
</commit_message>
<xml_diff>
--- a/Bill/Bill_Database.xlsx
+++ b/Bill/Bill_Database.xlsx
@@ -8,14 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SRCL\Bill\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE9DCD34-CE68-4B8D-9199-50FD95913ED7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6A67467-7350-40B5-9BD8-BE1EE1CB4F9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Advance" sheetId="1" r:id="rId1"/>
     <sheet name="Expense" sheetId="2" r:id="rId2"/>
     <sheet name="Salary" sheetId="3" r:id="rId3"/>
+    <sheet name="Food" sheetId="4" r:id="rId4"/>
+    <sheet name="Vouchers" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="151">
   <si>
     <t>Date</t>
   </si>
@@ -249,15 +251,9 @@
     <t>End of 2020, total advance received = 35180</t>
   </si>
   <si>
-    <t>End of 2020, total expense = 34925</t>
-  </si>
-  <si>
     <t>Mymensingh PWD + Tarakanda Park Report</t>
   </si>
   <si>
-    <t>Toner (M12a) + mouse Pad</t>
-  </si>
-  <si>
     <t>Transport + Breakfast</t>
   </si>
   <si>
@@ -276,10 +272,253 @@
     <t>December</t>
   </si>
   <si>
-    <t>January</t>
-  </si>
-  <si>
-    <t>February</t>
+    <t>End of 2020, total expense done = 34925</t>
+  </si>
+  <si>
+    <t>End of 2020, the remaining account balance = 255</t>
+  </si>
+  <si>
+    <t>Toner (M12a) + Mouse Pad</t>
+  </si>
+  <si>
+    <t>Adjustment</t>
+  </si>
+  <si>
+    <t>Tissue + Snacks</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Sl.</t>
+  </si>
+  <si>
+    <t>End of 2020</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Sweets</t>
+  </si>
+  <si>
+    <t>Courier to Imam, Mymensingh PWD</t>
+  </si>
+  <si>
+    <t>Table, Chair</t>
+  </si>
+  <si>
+    <t>Company</t>
+  </si>
+  <si>
+    <t>Unite Furniture</t>
+  </si>
+  <si>
+    <t>Furniture</t>
+  </si>
+  <si>
+    <t>Stationary Items</t>
+  </si>
+  <si>
+    <t>Sifat Trading</t>
+  </si>
+  <si>
+    <t>Crokaries</t>
+  </si>
+  <si>
+    <t>Mehedi Enterprise</t>
+  </si>
+  <si>
+    <t>Lizol</t>
+  </si>
+  <si>
+    <t>Siyam Enterprise</t>
+  </si>
+  <si>
+    <t>Washroom Accessories</t>
+  </si>
+  <si>
+    <t>Electronics Item</t>
+  </si>
+  <si>
+    <t>Maa Electronics</t>
+  </si>
+  <si>
+    <t>Carpet</t>
+  </si>
+  <si>
+    <t>Nakshi Carpet</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>Khan Agency &amp; Paint</t>
+  </si>
+  <si>
+    <t>Book</t>
+  </si>
+  <si>
+    <t>Islamic Foundation</t>
+  </si>
+  <si>
+    <t>Emarat Builders</t>
+  </si>
+  <si>
+    <t>RJSC</t>
+  </si>
+  <si>
+    <t>Harisson &amp; Company</t>
+  </si>
+  <si>
+    <t>Conference</t>
+  </si>
+  <si>
+    <t>ICWFM</t>
+  </si>
+  <si>
+    <t>Room</t>
+  </si>
+  <si>
+    <t>Hotel Payra</t>
+  </si>
+  <si>
+    <t>Visiting Card</t>
+  </si>
+  <si>
+    <t>Rupashi Bangla</t>
+  </si>
+  <si>
+    <t>Food &amp; Snacks</t>
+  </si>
+  <si>
+    <t>The Curry House</t>
+  </si>
+  <si>
+    <t>Khana Pina</t>
+  </si>
+  <si>
+    <t>New Nabanna Restaurant</t>
+  </si>
+  <si>
+    <t>Hot &amp; Tasty</t>
+  </si>
+  <si>
+    <t>Hardware</t>
+  </si>
+  <si>
+    <t>New Janata Hardware</t>
+  </si>
+  <si>
+    <t>Internet</t>
+  </si>
+  <si>
+    <t>Net2BD</t>
+  </si>
+  <si>
+    <t>Pan Pacific Sonargaon</t>
+  </si>
+  <si>
+    <t>Chair</t>
+  </si>
+  <si>
+    <t>Panthapeak Foreign Furniture</t>
+  </si>
+  <si>
+    <t>Gloria Jeans</t>
+  </si>
+  <si>
+    <t>LED Lights</t>
+  </si>
+  <si>
+    <t>Hossain Electric</t>
+  </si>
+  <si>
+    <t>Star Hotel &amp; Kabab</t>
+  </si>
+  <si>
+    <t>Air Bud</t>
+  </si>
+  <si>
+    <t>Gadget Studio</t>
+  </si>
+  <si>
+    <t>Banner</t>
+  </si>
+  <si>
+    <t>Digital Press Point</t>
+  </si>
+  <si>
+    <t>Coffee Cooker</t>
+  </si>
+  <si>
+    <t>Purnima Restaurant</t>
+  </si>
+  <si>
+    <t>Courier To Maksuda Apu</t>
+  </si>
+  <si>
+    <t>Sundarban</t>
+  </si>
+  <si>
+    <t>File Cabinet</t>
+  </si>
+  <si>
+    <t>SR Foreign Furniture</t>
+  </si>
+  <si>
+    <t>Chin Chin Chinese</t>
+  </si>
+  <si>
+    <t>The Manhattan Fish Market</t>
+  </si>
+  <si>
+    <t>Sor Gorom Restaurant</t>
+  </si>
+  <si>
+    <t>Euro Garden Restaurant</t>
+  </si>
+  <si>
+    <t>New Cathay</t>
+  </si>
+  <si>
+    <t>Hotel Swiss Garden</t>
+  </si>
+  <si>
+    <t>Coffee</t>
+  </si>
+  <si>
+    <t>Computer Accessories</t>
+  </si>
+  <si>
+    <t>RS Computers System</t>
+  </si>
+  <si>
+    <t>DHK-CTG-DHK Air Ticket</t>
+  </si>
+  <si>
+    <t>US Bangla Airlines</t>
+  </si>
+  <si>
+    <t>Ryans Computer</t>
+  </si>
+  <si>
+    <t>Account Deposit</t>
+  </si>
+  <si>
+    <t>Sonali Bank - 0440434291104</t>
+  </si>
+  <si>
+    <t>DBBL - 10715174320</t>
+  </si>
+  <si>
+    <t>EBL - 4037400000412586</t>
+  </si>
+  <si>
+    <t>Star Tech</t>
+  </si>
+  <si>
+    <t>Bikrampur Mistanno</t>
   </si>
 </sst>
 </file>
@@ -289,7 +528,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -342,6 +581,20 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0070C0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -357,7 +610,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -420,11 +673,48 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -442,35 +732,69 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -482,21 +806,38 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -945,13 +1286,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="25" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="11" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" style="1" customWidth="1"/>
     <col min="3" max="5" width="17.140625" style="1" customWidth="1"/>
     <col min="6" max="6" width="16.28515625" style="1" customWidth="1"/>
@@ -959,17 +1300,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="26" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="5"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -1237,31 +1578,31 @@
     </row>
     <row r="17" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="6"/>
-      <c r="B17" s="21" t="s">
+      <c r="B17" s="27" t="s">
         <v>60</v>
       </c>
-      <c r="C17" s="22"/>
-      <c r="D17" s="23"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="6"/>
-      <c r="B18" s="18" t="s">
-        <v>61</v>
-      </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="20"/>
+      <c r="B18" s="30" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
       <c r="E18" s="2"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
-      <c r="B19" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C19" s="16"/>
-      <c r="D19" s="17"/>
+      <c r="B19" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="C19" s="34"/>
+      <c r="D19" s="35"/>
       <c r="E19" s="2"/>
       <c r="F19" s="3"/>
     </row>
@@ -1274,55 +1615,75 @@
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="6">
+      <c r="A21" s="7">
         <v>44201</v>
       </c>
-      <c r="B21" s="26" t="s">
-        <v>62</v>
-      </c>
-      <c r="C21" s="2">
+      <c r="B21" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" s="3">
         <v>2000</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="E21" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="6">
+      <c r="A22" s="7">
         <v>44202</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>1000</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="3" t="s">
         <v>8</v>
       </c>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="6"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="2"/>
-      <c r="D23" s="2"/>
-      <c r="E23" s="2"/>
+      <c r="A23" s="6">
+        <v>44205</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2000</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="6"/>
-      <c r="B24" s="2"/>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
+      <c r="A24" s="6">
+        <v>44206</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2">
+        <v>500</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1549,47 +1910,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05325F8F-BEEC-4CC8-B184-0C8693CC2175}">
-  <dimension ref="A1:F50"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G54" sqref="G54"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="28.5703125" customWidth="1"/>
-    <col min="3" max="5" width="17.140625" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="28.5703125" style="3" customWidth="1"/>
+    <col min="3" max="5" width="17.140625" style="3" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="36" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="E2" s="7" t="s">
+      <c r="E2" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>44138</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1604,10 +1966,8 @@
       <c r="E3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
       <c r="B4" s="3" t="s">
         <v>14</v>
       </c>
@@ -1620,12 +1980,12 @@
       <c r="E4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="12">
+      <c r="F4" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="8">
+      <c r="A5" s="7">
         <v>44139</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1640,10 +2000,8 @@
       <c r="E5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F5" s="12"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
       <c r="B6" s="3" t="s">
         <v>15</v>
       </c>
@@ -1656,652 +2014,598 @@
       <c r="E6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="F6" s="12"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>44141</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="3">
         <v>65</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="3">
         <v>70</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="12"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="8">
+      <c r="A8" s="7">
         <v>44143</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="3">
         <v>30</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="3">
         <v>40</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="12"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="8">
+      <c r="A9" s="7">
         <v>44144</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="3">
         <v>100</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="3">
         <v>440</v>
       </c>
-      <c r="E9" s="2"/>
       <c r="F9" s="3">
         <v>500</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="8">
+      <c r="A10" s="7">
         <v>44145</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C10" s="2">
+      <c r="C10" s="3">
         <v>135</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D10" s="3">
         <v>305</v>
       </c>
-      <c r="E10" s="2"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="2">
+      <c r="C11" s="3">
         <v>150</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D11" s="3">
         <v>155</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="12"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C12" s="2">
+      <c r="C12" s="3">
         <v>30</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D12" s="3">
         <v>125</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="12"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="8">
+      <c r="A13" s="7">
         <v>44147</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="C13" s="2">
+      <c r="C13" s="3">
         <v>50</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D13" s="3">
         <v>75</v>
       </c>
-      <c r="E13" s="2"/>
       <c r="F13" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="8">
+      <c r="A14" s="7">
         <v>44156</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="2">
+      <c r="C14" s="3">
         <v>660</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D14" s="3">
         <v>415</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="12"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8">
+      <c r="A15" s="7">
         <v>44158</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C15" s="2">
+      <c r="C15" s="3">
         <v>275</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D15" s="3">
         <v>140</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="12"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8"/>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C16" s="2">
+      <c r="C16" s="3">
         <v>80</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D16" s="3">
         <v>60</v>
       </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="12"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>44171</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C17" s="2">
+      <c r="C17" s="3">
         <v>790</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D17" s="3">
         <v>1270</v>
       </c>
-      <c r="E17" s="2"/>
       <c r="F17" s="3">
         <v>2000</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="2">
+      <c r="C18" s="3">
         <v>680</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D18" s="3">
         <v>590</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="12"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="2">
+      <c r="C19" s="3">
         <v>205</v>
       </c>
-      <c r="D19" s="2">
+      <c r="D19" s="3">
         <v>385</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="12"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="8">
+      <c r="A20" s="7">
         <v>44172</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C20" s="2">
+      <c r="C20" s="3">
         <v>220</v>
       </c>
-      <c r="D20" s="2">
+      <c r="D20" s="3">
         <v>665</v>
       </c>
-      <c r="E20" s="2"/>
       <c r="F20" s="3">
         <v>500</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C21" s="2">
+      <c r="C21" s="3">
         <v>330</v>
       </c>
-      <c r="D21" s="2">
+      <c r="D21" s="3">
         <v>335</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="12"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C22" s="2">
+      <c r="C22" s="3">
         <v>230</v>
       </c>
-      <c r="D22" s="2">
+      <c r="D22" s="3">
         <v>105</v>
       </c>
-      <c r="E22" s="2"/>
-      <c r="F22" s="12">
+      <c r="F22" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="8">
+      <c r="A23" s="7">
         <v>44174</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C23" s="2">
+      <c r="C23" s="3">
         <v>850</v>
       </c>
-      <c r="D23" s="2">
+      <c r="D23" s="3">
         <v>255</v>
       </c>
-      <c r="E23" s="2"/>
       <c r="F23" s="3">
         <v>6250</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="2">
+      <c r="C24" s="3">
         <v>130</v>
       </c>
-      <c r="D24" s="2">
+      <c r="D24" s="3">
         <v>125</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="12"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="2">
+      <c r="C25" s="3">
         <v>120</v>
       </c>
-      <c r="D25" s="2">
+      <c r="D25" s="3">
         <v>5</v>
       </c>
-      <c r="E25" s="2"/>
-      <c r="F25" s="12"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C26" s="2">
+      <c r="C26" s="3">
         <v>310</v>
       </c>
-      <c r="D26" s="2">
+      <c r="D26" s="3">
         <v>-305</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="12">
+      <c r="F26" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="8">
+      <c r="A27" s="7">
         <v>44177</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C27" s="2">
+      <c r="C27" s="3">
         <v>6000</v>
       </c>
-      <c r="D27" s="2">
+      <c r="D27" s="3">
         <v>-55</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="12"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C28" s="2">
+      <c r="C28" s="3">
         <v>700</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D28" s="3">
         <v>-755</v>
       </c>
-      <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C29" s="2">
+      <c r="C29" s="3">
         <v>80</v>
       </c>
-      <c r="D29" s="2">
+      <c r="D29" s="3">
         <v>-835</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="12"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="8">
+      <c r="A30" s="7">
         <v>44180</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="2">
+      <c r="C30" s="3">
         <v>150</v>
       </c>
-      <c r="D30" s="2">
+      <c r="D30" s="3">
         <v>15</v>
       </c>
-      <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+      <c r="A31" s="7">
         <v>44182</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="2">
+      <c r="C31" s="3">
         <v>225</v>
       </c>
-      <c r="D31" s="2">
+      <c r="D31" s="3">
         <v>790</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="12">
+      <c r="F31" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="2">
+      <c r="C32" s="3">
         <v>390</v>
       </c>
-      <c r="D32" s="2">
+      <c r="D32" s="3">
         <v>400</v>
       </c>
-      <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C33" s="2">
+      <c r="C33" s="3">
         <v>200</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D33" s="3">
         <v>200</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" s="6">
+      <c r="A34" s="7">
         <v>44186</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="2">
+      <c r="C34" s="3">
         <v>610</v>
       </c>
-      <c r="D34" s="2">
+      <c r="D34" s="3">
         <v>590</v>
       </c>
-      <c r="E34" s="2"/>
       <c r="F34" s="3">
         <v>1000</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" s="6">
+      <c r="A35" s="7">
         <v>44188</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="2">
+      <c r="C35" s="3">
         <v>300</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D35" s="3">
         <v>290</v>
       </c>
-      <c r="E35" s="2"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
-      <c r="B36" s="2" t="s">
+      <c r="B36" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="2">
+      <c r="C36" s="3">
         <v>150</v>
       </c>
-      <c r="D36" s="2">
+      <c r="D36" s="3">
         <v>2140</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="12">
+      <c r="F36" s="3">
         <v>2000</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" s="6">
+      <c r="A37" s="7">
         <v>44189</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="C37" s="2">
+      <c r="C37" s="3">
         <v>1245</v>
       </c>
-      <c r="D37" s="2">
+      <c r="D37" s="3">
         <v>895</v>
       </c>
-      <c r="E37" s="2"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="6">
+      <c r="A38" s="7">
         <v>44190</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C38" s="2">
+      <c r="C38" s="3">
         <v>110</v>
       </c>
-      <c r="D38" s="2">
+      <c r="D38" s="3">
         <v>785</v>
       </c>
-      <c r="E38" s="2"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A39" s="6">
+      <c r="A39" s="7">
         <v>44194</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C39" s="2">
+      <c r="C39" s="3">
         <v>235</v>
       </c>
-      <c r="D39" s="2">
+      <c r="D39" s="3">
         <v>550</v>
       </c>
-      <c r="E39" s="2"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C40" s="2">
+      <c r="C40" s="3">
         <v>70</v>
       </c>
-      <c r="D40" s="2">
+      <c r="D40" s="3">
         <v>480</v>
       </c>
-      <c r="E40" s="2"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C41" s="2">
+      <c r="C41" s="3">
         <v>55</v>
       </c>
-      <c r="D41" s="2">
+      <c r="D41" s="3">
         <v>425</v>
       </c>
-      <c r="E41" s="2"/>
     </row>
     <row r="42" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="6">
+      <c r="A42" s="7">
         <v>44196</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42" s="3">
         <v>170</v>
       </c>
-      <c r="D42" s="2">
+      <c r="D42" s="3">
         <v>255</v>
       </c>
-      <c r="E42" s="2"/>
     </row>
     <row r="43" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="6"/>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="C43" s="16"/>
-      <c r="D43" s="17"/>
-      <c r="E43" s="2"/>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
+      <c r="C43" s="39"/>
+      <c r="D43" s="40"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A45" s="6">
+      <c r="A45" s="7">
         <v>44202</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C45" s="3">
+        <v>600</v>
+      </c>
+      <c r="D45" s="3">
+        <v>2655</v>
+      </c>
+      <c r="F45" s="3">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C46" s="3">
+        <v>105</v>
+      </c>
+      <c r="D46" s="3">
+        <v>2550</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="2">
-        <v>600</v>
-      </c>
-      <c r="D45" s="2">
-        <v>2655</v>
-      </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="2">
-        <v>3000</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
-      <c r="B46" s="2" t="s">
+      <c r="C47" s="3">
+        <v>2830</v>
+      </c>
+      <c r="D47" s="3">
+        <v>-280</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C46" s="2">
-        <v>105</v>
-      </c>
-      <c r="D46" s="2">
-        <v>2550</v>
-      </c>
-      <c r="E46" s="2"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
-      <c r="B47" s="2" t="s">
+      <c r="C48" s="3">
+        <v>260</v>
+      </c>
+      <c r="D48" s="3">
+        <v>-540</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C47" s="2">
-        <v>2830</v>
-      </c>
-      <c r="D47" s="2">
-        <v>-280</v>
-      </c>
-      <c r="E47" s="2"/>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
-      <c r="B48" s="2" t="s">
+      <c r="C49" s="3">
+        <v>510</v>
+      </c>
+      <c r="D49" s="3">
+        <v>-1050</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C48" s="2">
-        <v>260</v>
-      </c>
-      <c r="D48" s="2">
-        <v>-540</v>
-      </c>
-      <c r="E48" s="2"/>
-    </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="C49" s="2">
-        <v>510</v>
-      </c>
-      <c r="D49" s="2">
-        <v>-1050</v>
-      </c>
-    </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C50" s="2">
+      <c r="C50" s="3">
         <v>820</v>
       </c>
-      <c r="D50" s="2">
+      <c r="D50" s="3">
         <v>-1870</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="7">
+        <v>44205</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C51" s="3">
+        <v>2000</v>
+      </c>
+      <c r="D51" s="3">
+        <v>130</v>
+      </c>
+      <c r="F51" s="3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="7">
+        <v>44206</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C52" s="3">
+        <v>95</v>
+      </c>
+      <c r="D52" s="3">
+        <v>535</v>
       </c>
     </row>
   </sheetData>
@@ -2317,30 +2621,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BA63613-3F5D-49A3-B999-29B72C606D8C}">
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="17.140625" style="9" customWidth="1"/>
     <col min="2" max="2" width="28.5703125" customWidth="1"/>
     <col min="3" max="5" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="58.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+      <c r="A2" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="4" t="s">
@@ -2357,7 +2661,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="8">
+      <c r="A3" s="7">
         <v>44077</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -2374,11 +2678,9 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="9">
+      <c r="A4" s="7"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="8">
         <v>35000</v>
       </c>
       <c r="D4" s="3" t="s">
@@ -2389,10 +2691,8 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="8"/>
-      <c r="B5" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="A5" s="7"/>
+      <c r="B5" s="3"/>
       <c r="C5" s="3">
         <v>3000</v>
       </c>
@@ -2404,10 +2704,8 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="A6" s="7"/>
+      <c r="B6" s="3"/>
       <c r="C6" s="3">
         <v>10000</v>
       </c>
@@ -2419,7 +2717,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="8">
+      <c r="A7" s="7">
         <v>44107</v>
       </c>
       <c r="B7" s="3" t="s">
@@ -2436,10 +2734,8 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="8"/>
-      <c r="B8" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A8" s="7"/>
+      <c r="B8" s="3"/>
       <c r="C8" s="3">
         <v>35000</v>
       </c>
@@ -2451,10 +2747,8 @@
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A9" s="7"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="3">
         <v>3000</v>
       </c>
@@ -2466,10 +2760,8 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="8"/>
-      <c r="B10" s="3" t="s">
-        <v>23</v>
-      </c>
+      <c r="A10" s="7"/>
+      <c r="B10" s="3"/>
       <c r="C10" s="3">
         <v>8000</v>
       </c>
@@ -2481,7 +2773,7 @@
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+      <c r="A11" s="7">
         <v>44138</v>
       </c>
       <c r="B11" s="3" t="s">
@@ -2498,10 +2790,8 @@
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
-      <c r="B12" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A12" s="7"/>
+      <c r="B12" s="3"/>
       <c r="C12" s="3">
         <v>35000</v>
       </c>
@@ -2513,10 +2803,8 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A13" s="7"/>
+      <c r="B13" s="3"/>
       <c r="C13" s="3">
         <v>3000</v>
       </c>
@@ -2528,10 +2816,8 @@
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="8"/>
-      <c r="B14" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A14" s="7"/>
+      <c r="B14" s="3"/>
       <c r="C14" s="3">
         <v>5000</v>
       </c>
@@ -2543,10 +2829,8 @@
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="A15" s="7"/>
+      <c r="B15" s="3"/>
       <c r="C15" s="3">
         <v>3000</v>
       </c>
@@ -2558,7 +2842,7 @@
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+      <c r="A16" s="7">
         <v>44141</v>
       </c>
       <c r="B16" s="3" t="s">
@@ -2575,7 +2859,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="8">
+      <c r="A17" s="7">
         <v>44172</v>
       </c>
       <c r="B17" s="3" t="s">
@@ -2592,10 +2876,8 @@
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="8"/>
-      <c r="B18" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="A18" s="7"/>
+      <c r="B18" s="3"/>
       <c r="C18" s="3">
         <v>35000</v>
       </c>
@@ -2607,10 +2889,8 @@
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="A19" s="7"/>
+      <c r="B19" s="3"/>
       <c r="C19" s="3">
         <v>12000</v>
       </c>
@@ -2622,10 +2902,8 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="8"/>
-      <c r="B20" s="3" t="s">
-        <v>49</v>
-      </c>
+      <c r="A20" s="7"/>
+      <c r="B20" s="3"/>
       <c r="C20" s="3">
         <v>3000</v>
       </c>
@@ -2637,240 +2915,248 @@
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+      <c r="A21" s="7"/>
+      <c r="B21" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="C21" s="19">
+        <f>SUM(C3:C20)</f>
+        <v>271000</v>
+      </c>
+      <c r="D21" s="17"/>
+      <c r="E21" s="17"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>44201</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C21" s="3">
+      <c r="B22" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="3">
         <v>30000</v>
       </c>
-      <c r="D21" s="3" t="s">
+      <c r="D22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="8"/>
-      <c r="B22" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="C22" s="3">
+      <c r="E22" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="7"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3">
         <v>12000</v>
       </c>
-      <c r="D22" s="3" t="s">
+      <c r="D23" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
-      <c r="B23" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C23" s="3">
+      <c r="E23" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="7"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3">
         <v>3000</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="D24" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="8"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="E24" s="3" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="8"/>
+      <c r="A25" s="7"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" s="8"/>
+      <c r="A26" s="7"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="8"/>
+      <c r="A27" s="7"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="8"/>
+      <c r="A28" s="7"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="8"/>
+      <c r="A29" s="7"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="8"/>
+      <c r="A30" s="7"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="8"/>
+      <c r="A31" s="7"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="8"/>
+      <c r="A32" s="7"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="8"/>
+      <c r="A33" s="7"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="8"/>
+      <c r="A35" s="7"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="8"/>
+      <c r="A36" s="7"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
+      <c r="A37" s="7"/>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
       <c r="E37" s="3"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
+      <c r="A38" s="7"/>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
       <c r="D38" s="3"/>
       <c r="E38" s="3"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
+      <c r="A39" s="7"/>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
       <c r="E39" s="3"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
+      <c r="A40" s="7"/>
       <c r="B40" s="3"/>
       <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
+      <c r="A41" s="7"/>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
       <c r="E41" s="3"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
+      <c r="A42" s="7"/>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
       <c r="D42" s="3"/>
       <c r="E42" s="3"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
+      <c r="A43" s="7"/>
       <c r="B43" s="3"/>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
       <c r="E43" s="3"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
+      <c r="A44" s="7"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
       <c r="D44" s="3"/>
       <c r="E44" s="3"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
+      <c r="A45" s="7"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
       <c r="E45" s="3"/>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
+      <c r="A46" s="7"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
+      <c r="A47" s="7"/>
       <c r="B47" s="3"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
       <c r="E47" s="3"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
+      <c r="A48" s="7"/>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
       <c r="D48" s="3"/>
       <c r="E48" s="3"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
+      <c r="A49" s="7"/>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
       <c r="E49" s="3"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="8"/>
+      <c r="A50" s="7"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
       <c r="D50" s="3"/>
       <c r="E50" s="3"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="7"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2878,6 +3164,1309 @@
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECA08264-5F87-4633-B719-FCEF1F6ED1CC}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L18" sqref="L18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" style="13" customWidth="1"/>
+    <col min="2" max="2" width="10.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="10.28515625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" style="12" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="13">
+        <v>44140</v>
+      </c>
+      <c r="B2" s="3">
+        <v>605</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="13">
+        <v>44156</v>
+      </c>
+      <c r="B3" s="3">
+        <v>1120</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="13">
+        <v>44197</v>
+      </c>
+      <c r="B4" s="3">
+        <v>560</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA9A66EE-D8F3-476E-BC1E-0104523F77D2}">
+  <dimension ref="A1:E104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="17"/>
+    <col min="2" max="2" width="14.5703125" style="7" customWidth="1"/>
+    <col min="3" max="4" width="36.28515625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="12.85546875" style="17" customWidth="1"/>
+    <col min="6" max="16384" width="9.140625" style="17"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="21" t="s">
+        <v>74</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="17">
+        <v>1</v>
+      </c>
+      <c r="B2" s="7">
+        <v>42398</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="17">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="17">
+        <v>2</v>
+      </c>
+      <c r="B3" s="7">
+        <v>42398</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>82</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="17">
+        <v>5200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="17">
+        <v>3</v>
+      </c>
+      <c r="B4" s="7">
+        <v>42399</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="17">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="17">
+        <v>4</v>
+      </c>
+      <c r="B5" s="7">
+        <v>42399</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1708</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="17">
+        <v>5</v>
+      </c>
+      <c r="B6" s="7">
+        <v>42399</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1818</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="17">
+        <v>6</v>
+      </c>
+      <c r="B7" s="7">
+        <v>42399</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>83</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="17">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="17">
+        <v>7</v>
+      </c>
+      <c r="B8" s="7">
+        <v>42399</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="17">
+        <v>8</v>
+      </c>
+      <c r="B9" s="7">
+        <v>42399</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9" s="17">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" s="17">
+        <v>9</v>
+      </c>
+      <c r="B10" s="7">
+        <v>42399</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E10" s="17">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="17">
+        <v>10</v>
+      </c>
+      <c r="B11" s="7">
+        <v>42401</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="E11" s="17">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="17">
+        <v>11</v>
+      </c>
+      <c r="B12" s="7">
+        <v>42401</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="17">
+        <v>4750</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="17">
+        <v>12</v>
+      </c>
+      <c r="B13" s="7">
+        <v>42401</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>86</v>
+      </c>
+      <c r="E13" s="17">
+        <v>510</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
+        <v>13</v>
+      </c>
+      <c r="B14" s="7">
+        <v>42402</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="D14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="E14" s="17">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
+        <v>14</v>
+      </c>
+      <c r="B15" s="7">
+        <v>42404</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" s="17">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="17">
+        <v>15</v>
+      </c>
+      <c r="B16" s="7">
+        <v>42418</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>90</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="E16" s="17">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="7">
+        <v>42429</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E17" s="17">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <v>17</v>
+      </c>
+      <c r="B18" s="7">
+        <v>42403</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="17">
+        <v>24900</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="17">
+        <v>18</v>
+      </c>
+      <c r="B19" s="7">
+        <v>42753</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="17">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="17">
+        <v>19</v>
+      </c>
+      <c r="B20" s="7">
+        <v>43221</v>
+      </c>
+      <c r="C20" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="E20" s="17">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="17">
+        <v>20</v>
+      </c>
+      <c r="B21" s="7">
+        <v>43848</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="D21" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="E21" s="17">
+        <v>3100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="17">
+        <v>21</v>
+      </c>
+      <c r="B22" s="7">
+        <v>43858</v>
+      </c>
+      <c r="C22" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E22" s="17">
+        <v>3248</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="17">
+        <v>22</v>
+      </c>
+      <c r="B23" s="7">
+        <v>43860</v>
+      </c>
+      <c r="C23" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="E23" s="17">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <v>23</v>
+      </c>
+      <c r="B24" s="7">
+        <v>43862</v>
+      </c>
+      <c r="C24" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="E24" s="20">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="17">
+        <v>24</v>
+      </c>
+      <c r="B25" s="7">
+        <v>43863</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D25" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E25" s="17">
+        <v>810</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="17">
+        <v>25</v>
+      </c>
+      <c r="B26" s="7">
+        <v>43863</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E26" s="17">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <v>26</v>
+      </c>
+      <c r="B27" s="7">
+        <v>43863</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>111</v>
+      </c>
+      <c r="E27" s="17">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <v>27</v>
+      </c>
+      <c r="B28" s="7">
+        <v>43879</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="E28" s="17">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <v>28</v>
+      </c>
+      <c r="B29" s="7">
+        <v>43905</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="D29" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="E29" s="17">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
+        <v>29</v>
+      </c>
+      <c r="B30" s="7">
+        <v>44054</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="E30" s="17">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
+        <v>30</v>
+      </c>
+      <c r="B31" s="7">
+        <v>44088</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D31" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E31" s="17">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="17">
+        <v>31</v>
+      </c>
+      <c r="B32" s="7">
+        <v>44090</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D32" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E32" s="17">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
+        <v>32</v>
+      </c>
+      <c r="B33" s="7">
+        <v>44098</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>120</v>
+      </c>
+      <c r="D33" s="13" t="s">
+        <v>121</v>
+      </c>
+      <c r="E33" s="17">
+        <v>2200</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <v>33</v>
+      </c>
+      <c r="B34" s="7">
+        <v>44144</v>
+      </c>
+      <c r="C34" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D34" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="E34" s="17">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <v>34</v>
+      </c>
+      <c r="B35" s="7">
+        <v>44146</v>
+      </c>
+      <c r="C35" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="D35" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="E35" s="17">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <v>35</v>
+      </c>
+      <c r="B36" s="7">
+        <v>44156</v>
+      </c>
+      <c r="C36" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="D36" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="E36" s="17">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
+        <v>36</v>
+      </c>
+      <c r="B37" s="7">
+        <v>44166</v>
+      </c>
+      <c r="C37" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" s="13" t="s">
+        <v>127</v>
+      </c>
+      <c r="E37" s="17">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <v>37</v>
+      </c>
+      <c r="B38" s="7">
+        <v>44168</v>
+      </c>
+      <c r="C38" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="E38" s="17">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
+        <v>38</v>
+      </c>
+      <c r="B39" s="7">
+        <v>44172</v>
+      </c>
+      <c r="C39" s="13" t="s">
+        <v>129</v>
+      </c>
+      <c r="D39" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E39" s="17">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
+        <v>39</v>
+      </c>
+      <c r="B40" s="7">
+        <v>44174</v>
+      </c>
+      <c r="C40" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E40" s="17">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
+        <v>40</v>
+      </c>
+      <c r="B41" s="7">
+        <v>44186</v>
+      </c>
+      <c r="C41" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="13" t="s">
+        <v>133</v>
+      </c>
+      <c r="E41" s="17">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
+        <v>41</v>
+      </c>
+      <c r="B42" s="7">
+        <v>44179</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D42" s="13" t="s">
+        <v>149</v>
+      </c>
+      <c r="E42" s="17">
+        <v>9500</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
+        <v>42</v>
+      </c>
+      <c r="B43" s="7">
+        <v>43844</v>
+      </c>
+      <c r="C43" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="17">
+        <v>3020</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
+        <v>43</v>
+      </c>
+      <c r="B44" s="7">
+        <v>43881</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="13" t="s">
+        <v>135</v>
+      </c>
+      <c r="E44" s="17">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
+        <v>44</v>
+      </c>
+      <c r="B45" s="7">
+        <v>43875</v>
+      </c>
+      <c r="C45" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="13" t="s">
+        <v>136</v>
+      </c>
+      <c r="E45" s="17">
+        <v>1475</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="17">
+        <v>45</v>
+      </c>
+      <c r="B46" s="7">
+        <v>43892</v>
+      </c>
+      <c r="C46" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D46" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="17">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="17">
+        <v>46</v>
+      </c>
+      <c r="B47" s="7">
+        <v>43898</v>
+      </c>
+      <c r="C47" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="D47" s="13" t="s">
+        <v>138</v>
+      </c>
+      <c r="E47" s="17">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="17">
+        <v>47</v>
+      </c>
+      <c r="B48" s="7">
+        <v>43906</v>
+      </c>
+      <c r="C48" s="13" t="s">
+        <v>139</v>
+      </c>
+      <c r="D48" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="E48" s="17">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="17">
+        <v>48</v>
+      </c>
+      <c r="B49" s="7">
+        <v>44088</v>
+      </c>
+      <c r="C49" s="13" t="s">
+        <v>142</v>
+      </c>
+      <c r="D49" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="E49" s="17">
+        <v>21592</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="17">
+        <v>49</v>
+      </c>
+      <c r="B50" s="7">
+        <v>44147</v>
+      </c>
+      <c r="C50" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="D50" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="E50" s="17">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
+        <v>50</v>
+      </c>
+      <c r="B51" s="7">
+        <v>44182</v>
+      </c>
+      <c r="C51" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="E51" s="17">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="17">
+        <v>51</v>
+      </c>
+      <c r="B52" s="7">
+        <v>44182</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D52" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="E52" s="17">
+        <v>10018</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="17">
+        <v>52</v>
+      </c>
+      <c r="B53" s="7">
+        <v>44182</v>
+      </c>
+      <c r="C53" s="13" t="s">
+        <v>145</v>
+      </c>
+      <c r="D53" s="13" t="s">
+        <v>147</v>
+      </c>
+      <c r="E53" s="17">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="42" t="s">
+        <v>75</v>
+      </c>
+      <c r="B54" s="43"/>
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="19">
+        <f>SUM(E2:E53)</f>
+        <v>158044</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="17">
+        <v>1</v>
+      </c>
+      <c r="B55" s="7">
+        <v>44201</v>
+      </c>
+      <c r="C55" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D55" s="13" t="s">
+        <v>150</v>
+      </c>
+      <c r="E55" s="17">
+        <v>1050</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
+        <v>2</v>
+      </c>
+      <c r="B56" s="7">
+        <v>44203</v>
+      </c>
+      <c r="C56" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D56" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E56" s="17">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="17">
+        <v>3</v>
+      </c>
+      <c r="B57" s="7">
+        <v>44203</v>
+      </c>
+      <c r="C57" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="D57" s="13" t="s">
+        <v>130</v>
+      </c>
+      <c r="E57" s="17">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" s="17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" s="17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" s="17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" s="17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="17">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="17">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="17">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="17">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="17">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="17">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="17">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="17">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="17">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="17">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="17">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="17">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="17">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="17">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="17">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A54:B54"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>